<commit_message>
Adiciona pasta Modulo_1 com exercícios iniciais
</commit_message>
<xml_diff>
--- a/Modulo_1/M1_Objetivo_Ciencia_De_Dados.xlsx
+++ b/Modulo_1/M1_Objetivo_Ciencia_De_Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Registro Diário" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Data</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Dificuldade Média</t>
-  </si>
-  <si>
-    <t>Vídeo - Leitura</t>
   </si>
 </sst>
 </file>
@@ -415,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -477,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -514,10 +511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,6 +552,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>